<commit_message>
[VM:Doug.Stearns@9/9/2014 1:15:46 PM] ecl phase 2 quality and supervisor updates
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13693
</commit_message>
<xml_diff>
--- a/Requirements/status_email_notify.xlsx
+++ b/Requirements/status_email_notify.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="77">
   <si>
     <t>CSR</t>
   </si>
@@ -72,9 +72,6 @@
     <t>NOT Quality Specialist Coaching</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>Pending Supervisor Review</t>
   </si>
   <si>
@@ -207,21 +204,9 @@
     <t>A new eCoaching Log has been entered and requires your action. Please click on the link below to review and verify that the eCL entered on &lt;strong&gt;" &amp; DateTime.Now().ToString &amp; "&lt;/strong&gt;"  for &lt;strong&gt;" &amp; strPerson &amp; "&lt;/strong&gt; is a valid Customer Service Escalation (CSE). Further directions are provided on the form.</t>
   </si>
   <si>
-    <t>A new eCoaching Log has been entered on behalf of &lt;strong&gt;" &amp; strPerson &amp; "&lt;/strong&gt;"  on &lt;strong&gt;" &amp; DateTime.Now().ToString &amp; "&lt;/strong&gt; that requires your action. Please click on the link below  to review the eCoaching log. After you have reviewed and coached an email will go to " &amp; strPerson &amp; " with direction to review and verify the coaching  opportunity.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A new eCoaching Log has been entered on your behalf. Please click on the link below to review and verify the coaching opportunity received on &lt;DATE&gt;. Opportunity. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">A new eCoaching Log has been entered on behalf of ToString &amp; “&lt;/strong&gt; on &lt;strong&gt;” &amp; DateTime.Now()  that requires your action. Please click on the link below to review the eCoaching log. After you have reviewed and coached an email will go to ToString &amp; “&lt;/strong with direction to review and verify the coaching opportunity. </t>
-  </si>
-  <si>
     <t xml:space="preserve">A new eCoaching Log has been entered and requires your action. Please click on the link below to review and verify that the eCL entered on &lt;DATE&gt; for &lt;EMPLOYEE NAME&gt;  is a valid Customer Service Escalation (CSE). Further directions are provided on the form. </t>
   </si>
   <si>
-    <t xml:space="preserve">A new eCoaching Log has been entered on behalf of &lt;EMPLOYEE NAME&gt; on &lt;DATE&gt; that requires your action. Please click on the link below to review the eCoaching log. After you have reviewed and coached an email will go to &lt;EMPLOYEE NAME&gt; with direction to review and verify the coaching opportunity. </t>
-  </si>
-  <si>
     <t>status after review</t>
   </si>
   <si>
@@ -231,13 +216,41 @@
     <t>Pending Acknowledgement</t>
   </si>
   <si>
-    <t xml:space="preserve">A new eCoaching Log has been entered on your behalf. Please click on the link below to review and verify the coaching opportunity received on &lt;DATE&gt;. </t>
-  </si>
-  <si>
     <t>eCL: Pending Acknowledgement (" &amp; strPerson &amp; ")</t>
   </si>
   <si>
     <t>Reinforcement, Met goal</t>
+  </si>
+  <si>
+    <t>A new eCoaching Log has been entered and requires your action. Please click on the link below to review and acknowledge the eCL entered on &lt;strong&gt;" &amp; Date &amp; "&lt;/strong&gt;" &amp; "Please click on the link below to review the eCoaching log.</t>
+  </si>
+  <si>
+    <t>Employee (CSR)
+Supervisor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A new eCoaching Log has been entered on your behalf. Please click on the link below to review and verify the coaching opportunity received on &lt;DATE&gt;. opportunity. </t>
+  </si>
+  <si>
+    <t>Supervisor
+If source NOT OMR send copy to Manager</t>
+  </si>
+  <si>
+    <t>Employee (Supervisor)
+Manager</t>
+  </si>
+  <si>
+    <t>Employee (Quality Specialist)
+Quality Lead</t>
+  </si>
+  <si>
+    <t>strSource in feed file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A new eCoaching Log has been entered on behalf of &lt;strong&gt;" &amp; strPerson &amp; "&lt;/strong&gt;"  on &lt;strong&gt;" &amp; DateTime.Now().ToString &amp; "&lt;/strong&gt; that requires your action. Please click on the link below  to review the eCoaching log. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A new eCoaching Log has been entered on behalf of &lt;EMPLOYEE NAME&gt; on &lt;DATE&gt; that requires your action. Please click on the link below to review the eCoaching log. </t>
   </si>
 </sst>
 </file>
@@ -416,46 +429,46 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,7 +772,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -776,33 +791,33 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="23"/>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -824,20 +839,20 @@
         <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="I7" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="32" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -850,21 +865,21 @@
         <v>9</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="29"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
@@ -878,18 +893,18 @@
         <v>13</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="29"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="17" t="s">
         <v>10</v>
       </c>
@@ -897,24 +912,24 @@
         <v>14</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="29"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="12" t="s">
         <v>6</v>
       </c>
@@ -922,56 +937,56 @@
         <v>17</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="29" t="s">
-        <v>21</v>
+    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="33"/>
+      <c r="B12" s="32" t="s">
+        <v>20</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="G12" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="29"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>12</v>
@@ -980,102 +995,102 @@
         <v>13</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
       <c r="B14" s="26"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="41"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="41"/>
+      <c r="H14" s="30"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="38" t="s">
-        <v>18</v>
+    <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>74</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>38</v>
+        <v>65</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="38"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="35"/>
       <c r="E16" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="38"/>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="33"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="35"/>
       <c r="E17" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>71</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H17" s="28" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="I17" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="38"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="35"/>
       <c r="E18" s="7" t="s">
         <v>12</v>
       </c>
@@ -1083,88 +1098,88 @@
         <v>13</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="29"/>
       <c r="B19" s="26"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="41"/>
+      <c r="H19" s="30"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>21</v>
+    <row r="20" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>20</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>20</v>
+        <v>65</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="29"/>
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="33"/>
+      <c r="B21" s="32"/>
       <c r="C21" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="33"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="I21" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="D22" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>12</v>
@@ -1173,13 +1188,13 @@
         <v>13</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1192,6 +1207,9 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A15:A18"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="B12:B13"/>
@@ -1199,9 +1217,6 @@
     <mergeCell ref="D15:D18"/>
     <mergeCell ref="C15:C18"/>
     <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A15:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1229,33 +1244,33 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="23"/>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
+      <c r="A6" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1277,208 +1292,208 @@
         <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="I7" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="29" t="s">
+      <c r="A8" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="32" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="7" t="s">
+      <c r="H8" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="29"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>24</v>
-      </c>
       <c r="G9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>45</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="29" t="s">
-        <v>21</v>
+      <c r="A10" s="33"/>
+      <c r="B10" s="32" t="s">
+        <v>20</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="29"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="17" t="s">
+      <c r="H11" s="18" t="s">
         <v>48</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>49</v>
       </c>
       <c r="I11" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>18</v>
+    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>74</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>24</v>
+        <v>65</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>72</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I12" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="34"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="15" t="s">
-        <v>24</v>
-      </c>
       <c r="G13" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="16" t="s">
         <v>44</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>45</v>
       </c>
       <c r="I13" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="34"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="38"/>
       <c r="E14" s="15" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="34"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="15" t="s">
+      <c r="H15" s="16" t="s">
         <v>48</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>49</v>
       </c>
       <c r="I15" s="15" t="s">
         <v>12</v>
@@ -1521,33 +1536,33 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="23"/>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
+      <c r="A6" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1569,211 +1584,211 @@
         <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="I7" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="35" t="s">
+      <c r="A8" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="41" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="G8" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="20" t="s">
-        <v>55</v>
-      </c>
       <c r="H8" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="20" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-      <c r="B9" s="35"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>45</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
-      <c r="B10" s="35" t="s">
-        <v>21</v>
+      <c r="A10" s="42"/>
+      <c r="B10" s="41" t="s">
+        <v>20</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="H10" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="42"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H10" s="13" t="s">
+      <c r="E11" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="20" t="s">
+      <c r="F11" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="G11" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="20" t="s">
-        <v>55</v>
-      </c>
       <c r="H11" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>28</v>
+    </row>
+    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>73</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I12" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="34"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G13" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="19" t="s">
         <v>44</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>45</v>
       </c>
       <c r="I13" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="34"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="38"/>
       <c r="E14" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>51</v>
-      </c>
       <c r="H14" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="34"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="G15" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="20" t="s">
-        <v>55</v>
-      </c>
       <c r="H15" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="20" t="s">
         <v>49</v>
-      </c>
-      <c r="I15" s="20" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[VM:Doug.Stearns@9/29/2014 11:46:14 AM] p13479 - ecl warning for csr TTuser/items:Doug Stearns(stead1) Resolution for SCCB-S13479.DV.1: Add WARNING question in the eCoaching Log (R&T) - Pending Dev - Doug Stearns
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13726
</commit_message>
<xml_diff>
--- a/Requirements/status_email_notify.xlsx
+++ b/Requirements/status_email_notify.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="82">
   <si>
     <t>CSR</t>
   </si>
@@ -254,6 +254,15 @@
   </si>
   <si>
     <t>P13515 - eCL eMail Mappings</t>
+  </si>
+  <si>
+    <t>P13479 - eCL Warning Log for CSR</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>Progressive Disciplinary Warning</t>
   </si>
 </sst>
 </file>
@@ -294,7 +303,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,8 +346,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -361,11 +376,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -422,9 +474,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -461,6 +510,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -762,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E5"/>
+  <dimension ref="B2:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,49 +855,49 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="28" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="31">
+      <c r="B3" s="30">
         <v>41869</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="32">
         <v>1</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="32" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="31">
+      <c r="B4" s="30">
         <v>41891</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="32">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="34" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="36">
+      <c r="B5" s="35">
         <v>41905</v>
       </c>
       <c r="C5" t="s">
@@ -829,6 +907,20 @@
         <v>1.2</v>
       </c>
       <c r="E5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="35">
+        <v>41908</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6">
+        <v>1.3</v>
+      </c>
+      <c r="E6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -839,64 +931,69 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="61" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="55.140625" customWidth="1"/>
-    <col min="10" max="10" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.140625" customWidth="1"/>
+    <col min="11" max="11" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" t="s">
         <v>45</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="E3" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="50"/>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -904,365 +1001,463 @@
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+    <row r="8" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="45" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>58</v>
-      </c>
       <c r="H8" s="9" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="J8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="37"/>
+    <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="43"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>58</v>
-      </c>
       <c r="H9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="J9" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="K9" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="37"/>
+    <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="43"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="E10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="F10" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="G10" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="15" t="s">
-        <v>58</v>
-      </c>
       <c r="H10" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="J10" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="K10" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="37"/>
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="43"/>
+      <c r="B11" s="47"/>
       <c r="C11" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="F11" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="G11" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>58</v>
-      </c>
       <c r="H11" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="J11" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="K11" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="37" t="s">
+    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="43"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="K12" s="48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="43"/>
+      <c r="B13" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="9" t="s">
+      <c r="H13" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="J13" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="K13" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="7" t="s">
+    <row r="14" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="43"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="G14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" s="7" t="s">
+      <c r="H14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="J14" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="K14" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="27" t="s">
+    <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="44"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="J15" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="K15" s="48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="19"/>
-      <c r="C16" s="4"/>
+      <c r="C16" s="41"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
+      <c r="I16" s="4"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B19" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C19" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="E19" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="F19" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="H19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="I19" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="J19" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="K19" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="38"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="12" t="s">
+    <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="37"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="E20" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="F20" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="G20" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="H18" s="12" t="s">
+      <c r="H20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="J20" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="K20" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="7" t="s">
+    <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="37"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="G21" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" s="7" t="s">
+      <c r="H21" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I21" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="J21" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="K21" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="A8:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B8:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1313,18 +1508,18 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1359,10 +1554,10 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="36" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -1391,8 +1586,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="37"/>
+      <c r="A9" s="37"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
@@ -1419,8 +1614,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="37" t="s">
+      <c r="A10" s="37"/>
+      <c r="B10" s="36" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="12" t="s">
@@ -1449,8 +1644,8 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="37"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="15" t="s">
         <v>10</v>
       </c>
@@ -1544,18 +1739,18 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1590,10 +1785,10 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -1622,8 +1817,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="28" t="s">
+      <c r="A9" s="39"/>
+      <c r="B9" s="27" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="12" t="s">

</xml_diff>

<commit_message>
[VM:Doug.Stearns@10/1/2014 9:04:58 AM] p13479 - ecl csr warning TTuser/items:Doug Stearns(stead1) Resolution for SCCB-S13479.DV.1: Add WARNING question in the eCoaching Log (R&T) - Verification and Validation - Doug Stearns
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13727
</commit_message>
<xml_diff>
--- a/Requirements/status_email_notify.xlsx
+++ b/Requirements/status_email_notify.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="82">
   <si>
     <t>CSR</t>
   </si>
@@ -417,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -499,46 +499,43 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -840,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E6"/>
+  <dimension ref="B2:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,6 +921,20 @@
         <v>76</v>
       </c>
     </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="35">
+        <v>41908</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7">
+        <v>1.4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -931,10 +942,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,7 +981,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
+      <c r="A3" s="40"/>
       <c r="B3" t="s">
         <v>81</v>
       </c>
@@ -979,19 +990,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1029,10 +1040,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="46" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -1064,7 +1075,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="47"/>
       <c r="C9" s="7" t="s">
         <v>6</v>
@@ -1095,7 +1106,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="47"/>
       <c r="C10" s="15" t="s">
         <v>6</v>
@@ -1126,7 +1137,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="47"/>
       <c r="C11" s="12" t="s">
         <v>6</v>
@@ -1157,39 +1168,39 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="48" t="s">
+      <c r="A12" s="45"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="48" t="s">
+      <c r="E12" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="48" t="s">
+      <c r="G12" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" s="48" t="s">
+      <c r="H12" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="49" t="s">
+      <c r="J12" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="K12" s="48" t="s">
+      <c r="K12" s="38" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
-      <c r="B13" s="45" t="s">
+      <c r="A13" s="45"/>
+      <c r="B13" s="46" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -1221,7 +1232,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="47"/>
       <c r="C14" s="7" t="s">
         <v>6</v>
@@ -1251,212 +1262,181 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="48" t="s">
+    <row r="15" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="48" t="s">
+      <c r="E16" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="42"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K19" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="I15" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="J15" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="K15" s="48" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="7" t="s">
+    </row>
+    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="42"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G20" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I17" s="7" t="s">
+      <c r="H20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="K17" s="7" t="s">
+      <c r="J20" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K20" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="K19" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="37"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="J20" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A18:A20"/>
     <mergeCell ref="A6:K6"/>
-    <mergeCell ref="A8:A15"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="B8:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1508,18 +1488,18 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1554,10 +1534,10 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="41" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -1586,8 +1566,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="36"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
@@ -1614,8 +1594,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="36" t="s">
+      <c r="A10" s="42"/>
+      <c r="B10" s="41" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="12" t="s">
@@ -1644,8 +1624,8 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
-      <c r="B11" s="36"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="41"/>
       <c r="C11" s="15" t="s">
         <v>10</v>
       </c>
@@ -1739,18 +1719,18 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1785,7 +1765,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="49" t="s">
         <v>70</v>
       </c>
       <c r="B8" s="27" t="s">
@@ -1817,7 +1797,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="27" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
[VM:Doug.Stearns@10/7/2014 3:30:48 PM] p13479 - ecl csr warnings TTuser/items:Doug Stearns(stead1) Resolution for SCCB-S13479.DV.1: Add WARNING question in the eCoaching Log (R&T) - Verification and Validation - Jourdain Augustin
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13729
</commit_message>
<xml_diff>
--- a/Requirements/status_email_notify.xlsx
+++ b/Requirements/status_email_notify.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="82">
   <si>
     <t>CSR</t>
   </si>
@@ -837,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E7"/>
+  <dimension ref="B2:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,6 +935,20 @@
         <v>76</v>
       </c>
     </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="35">
+        <v>41915</v>
+      </c>
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8">
+        <v>1.5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -945,7 +959,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,7 +1181,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="45"/>
       <c r="B12" s="48"/>
       <c r="C12" s="38" t="s">
@@ -1180,19 +1194,19 @@
         <v>58</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="G12" s="38" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H12" s="38" t="s">
         <v>58</v>
       </c>
       <c r="I12" s="38" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="J12" s="39" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="K12" s="38" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
[VM:Doug.Stearns@10/21/2014 11:18:02 AM] p13653 - ecl lsa module TTuser/items:Doug Stearns(stead1) Resolution for SCCB-S13653.DV.1: eCoaching - LSA Module (FS) - Pending Development - Doug Stearns
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13747
</commit_message>
<xml_diff>
--- a/Requirements/status_email_notify.xlsx
+++ b/Requirements/status_email_notify.xlsx
@@ -11,13 +11,14 @@
     <sheet name="CSR" sheetId="1" r:id="rId2"/>
     <sheet name="Supervisor" sheetId="2" r:id="rId3"/>
     <sheet name="Quality" sheetId="3" r:id="rId4"/>
+    <sheet name="LSA" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="92">
   <si>
     <t>CSR</t>
   </si>
@@ -263,6 +264,36 @@
   </si>
   <si>
     <t>Progressive Disciplinary Warning</t>
+  </si>
+  <si>
+    <t>LSA, LSA Manager, Desktop Manager</t>
+  </si>
+  <si>
+    <t>Employee (LSA)</t>
+  </si>
+  <si>
+    <t>LSA Manager</t>
+  </si>
+  <si>
+    <t>LSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P13653 - eCL LSA Module </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A new eCoaching Log has been entered on your behalf. Please click on the link below to review and verify the coaching opportunity received on &lt;DATE&gt;. </t>
+  </si>
+  <si>
+    <t>Pending Employee Review</t>
+  </si>
+  <si>
+    <t>eCL: Pending CSR Review (" &amp; strPerson &amp; ")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A new eCoaching Log has been entered on your behalf. Please click on the link below to review and verify the coaching opportunity received on &lt;DATE&gt;. Opportunity. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A new eCoaching Log has been entered on behalf of &lt;EMPLOYEE NAME&gt; on &lt;DATE&gt; that requires your action. Please click on the link below to review the eCoaching log. After you have reviewed and coached an email will go to &lt;EMPLOYEE NAME&gt; with direction to review and verify the coaching opportunity. </t>
   </si>
 </sst>
 </file>
@@ -303,7 +334,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +380,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -417,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -464,15 +501,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -498,9 +526,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -535,6 +560,31 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -837,64 +887,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E8"/>
+  <dimension ref="B2:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.28515625" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="25" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="30">
+      <c r="B3" s="27">
         <v>41869</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="29">
         <v>1</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="29" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="30">
+      <c r="B4" s="27">
         <v>41891</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="31" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="35">
+      <c r="B5" s="32">
         <v>41905</v>
       </c>
       <c r="C5" t="s">
@@ -908,7 +958,7 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="35">
+      <c r="B6" s="32">
         <v>41908</v>
       </c>
       <c r="C6" t="s">
@@ -922,7 +972,7 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="35">
+      <c r="B7" s="32">
         <v>41908</v>
       </c>
       <c r="C7" t="s">
@@ -936,7 +986,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="35">
+      <c r="B8" s="32">
         <v>41915</v>
       </c>
       <c r="C8" t="s">
@@ -946,6 +996,20 @@
         <v>1.5</v>
       </c>
       <c r="E8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="32">
+        <v>41929</v>
+      </c>
+      <c r="C9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9">
+        <v>1.6</v>
+      </c>
+      <c r="E9" t="s">
         <v>76</v>
       </c>
     </row>
@@ -956,11 +1020,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -995,7 +1057,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
+      <c r="A3" s="36"/>
       <c r="B3" t="s">
         <v>81</v>
       </c>
@@ -1004,19 +1066,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1054,10 +1116,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="42" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -1089,8 +1151,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="47"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="7" t="s">
         <v>6</v>
       </c>
@@ -1120,8 +1182,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
-      <c r="B10" s="47"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="43"/>
       <c r="C10" s="15" t="s">
         <v>6</v>
       </c>
@@ -1151,8 +1213,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
-      <c r="B11" s="47"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="43"/>
       <c r="C11" s="12" t="s">
         <v>6</v>
       </c>
@@ -1182,39 +1244,39 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="38" t="s">
+      <c r="A12" s="41"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="38" t="s">
+      <c r="E12" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" s="38" t="s">
+      <c r="H12" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="39" t="s">
+      <c r="J12" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="K12" s="38" t="s">
+      <c r="K12" s="34" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
-      <c r="B13" s="46" t="s">
+      <c r="A13" s="41"/>
+      <c r="B13" s="42" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -1246,8 +1308,8 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
-      <c r="B14" s="47"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="43"/>
       <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
@@ -1279,7 +1341,7 @@
     <row r="15" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
       <c r="B15" s="19"/>
-      <c r="C15" s="37"/>
+      <c r="C15" s="33"/>
       <c r="D15" s="4"/>
       <c r="E15" s="21"/>
       <c r="F15" s="4"/>
@@ -1289,169 +1351,249 @@
       <c r="J15" s="21"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+    <row r="16" spans="1:11" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="37" t="s">
+      <c r="C16" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="J16" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="K16" s="50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="J17" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="K17" s="50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="22" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="38"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" s="52" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="38"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G19" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I16" s="7" t="s">
+      <c r="H19" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J19" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="K19" s="46" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="4"/>
-    </row>
-    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="42" t="s">
+    <row r="20" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B21" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="9" t="s">
+      <c r="C21" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F21" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G21" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H21" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I21" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="J21" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="K18" s="12" t="s">
+      <c r="K21" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="12" t="s">
+    <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="38"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E22" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F22" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G22" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="I19" s="12" t="s">
+      <c r="H22" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I22" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="J22" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="K19" s="12" t="s">
+      <c r="K22" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="7" t="s">
+    <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="38"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E23" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G23" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I20" s="7" t="s">
+      <c r="H23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J23" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="K20" s="7" t="s">
+      <c r="K23" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A18:A20"/>
+  <mergeCells count="11">
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="A21:A23"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="A8:A14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B8:B12"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="E16:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1502,18 +1644,18 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1548,10 +1690,10 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="37" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -1580,8 +1722,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
-      <c r="B9" s="41"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
@@ -1608,8 +1750,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
-      <c r="B10" s="41" t="s">
+      <c r="A10" s="38"/>
+      <c r="B10" s="37" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="12" t="s">
@@ -1638,8 +1780,8 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
-      <c r="B11" s="41"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="15" t="s">
         <v>10</v>
       </c>
@@ -1693,9 +1835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1733,18 +1873,18 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1779,10 +1919,10 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="24" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -1811,8 +1951,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
-      <c r="B9" s="27" t="s">
+      <c r="A9" s="45"/>
+      <c r="B9" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="12" t="s">
@@ -1859,4 +1999,184 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.28515625" customWidth="1"/>
+    <col min="11" max="11" width="33" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="17"/>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="22"/>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="45"/>
+      <c r="B9" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="A8:A9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[VM:Doug.Stearns@10/31/2014 8:24:20 AM] p13659 - ecl ets data feed TTuser/items:Doug Stearns(stead1) Resolution for SCCB-S13659.DV.1: eCoaching - ETS data feed (FS) - Pending Development - Doug Stearns
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13782
</commit_message>
<xml_diff>
--- a/Requirements/status_email_notify.xlsx
+++ b/Requirements/status_email_notify.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="94">
   <si>
     <t>CSR</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t xml:space="preserve">A new eCoaching Log has been entered on behalf of &lt;EMPLOYEE NAME&gt; on &lt;DATE&gt; that requires your action. Please click on the link below to review the eCoaching log. After you have reviewed and coached an email will go to &lt;EMPLOYEE NAME&gt; with direction to review and verify the coaching opportunity. </t>
+  </si>
+  <si>
+    <t>P13659 - eCL ETS Data Feed</t>
+  </si>
+  <si>
+    <t>ETS</t>
   </si>
 </sst>
 </file>
@@ -454,19 +460,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -540,27 +539,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -578,6 +556,30 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -585,6 +587,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E9"/>
+  <dimension ref="B2:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,49 +907,49 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="22" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="27">
+      <c r="B3" s="24">
         <v>41869</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="26">
         <v>1</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="26" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="27">
+      <c r="B4" s="24">
         <v>41891</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="28" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="32">
+      <c r="B5" s="29">
         <v>41905</v>
       </c>
       <c r="C5" t="s">
@@ -958,7 +963,7 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="32">
+      <c r="B6" s="29">
         <v>41908</v>
       </c>
       <c r="C6" t="s">
@@ -972,7 +977,7 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="32">
+      <c r="B7" s="29">
         <v>41908</v>
       </c>
       <c r="C7" t="s">
@@ -986,7 +991,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="32">
+      <c r="B8" s="29">
         <v>41915</v>
       </c>
       <c r="C8" t="s">
@@ -1000,7 +1005,7 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="32">
+      <c r="B9" s="29">
         <v>41929</v>
       </c>
       <c r="C9" t="s">
@@ -1010,6 +1015,20 @@
         <v>1.6</v>
       </c>
       <c r="E9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="29">
+        <v>41942</v>
+      </c>
+      <c r="C10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10">
+        <v>1.7</v>
+      </c>
+      <c r="E10" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1020,9 +1039,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1039,7 +1060,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
+      <c r="A1" s="14"/>
       <c r="B1" t="s">
         <v>44</v>
       </c>
@@ -1048,7 +1069,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
+      <c r="A2" s="15"/>
       <c r="B2" t="s">
         <v>45</v>
       </c>
@@ -1057,7 +1078,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
+      <c r="A3" s="33"/>
       <c r="B3" t="s">
         <v>81</v>
       </c>
@@ -1066,19 +1087,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1116,470 +1137,508 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I8" s="9" t="s">
+      <c r="H8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="7" t="s">
+      <c r="A9" s="48"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="7" t="s">
+      <c r="H9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="15" t="s">
+      <c r="A10" s="48"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="15" t="s">
+      <c r="H10" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="12" t="s">
+      <c r="A11" s="48"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="I11" s="12" t="s">
+      <c r="H11" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="34" t="s">
+      <c r="A12" s="48"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="34" t="s">
+      <c r="E12" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="34" t="s">
+      <c r="G12" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" s="34" t="s">
+      <c r="H12" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="35" t="s">
+      <c r="J12" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="K12" s="34" t="s">
+      <c r="K12" s="31" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
-      <c r="B13" s="42" t="s">
+      <c r="A13" s="48"/>
+      <c r="B13" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" s="9" t="s">
+      <c r="H13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="J13" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="K13" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="7" t="s">
+      <c r="A14" s="48"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I14" s="7" t="s">
+      <c r="H14" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="K14" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="1:11" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+    <row r="15" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="54" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="55" t="s">
+      <c r="C16" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="56" t="s">
+      <c r="E16" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="48" t="s">
+      <c r="F16" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="G16" s="48" t="s">
+      <c r="G16" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="I16" s="48" t="s">
+      <c r="H16" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="J16" s="49" t="s">
+      <c r="J16" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="K16" s="50" t="s">
+      <c r="K16" s="40" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="50" t="s">
+    <row r="17" spans="1:11" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="45"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="G17" s="50" t="s">
+      <c r="G17" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="I17" s="50" t="s">
+      <c r="H17" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="J17" s="51" t="s">
+      <c r="J17" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="K17" s="50" t="s">
+      <c r="K17" s="40" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="22" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="38"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="52" t="s">
+    <row r="18" spans="1:11" s="19" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="45"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="52" t="s">
+      <c r="G18" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="52" t="s">
-        <v>58</v>
-      </c>
-      <c r="I18" s="52" t="s">
+      <c r="H18" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="J18" s="53" t="s">
+      <c r="J18" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="K18" s="52" t="s">
+      <c r="K18" s="42" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="46" t="s">
+      <c r="A19" s="45"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="46" t="s">
+      <c r="G19" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="I19" s="46" t="s">
+      <c r="H19" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="47" t="s">
+      <c r="J19" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="K19" s="46" t="s">
+      <c r="K19" s="36" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="4"/>
+    <row r="20" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="9" t="s">
+      <c r="C21" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I21" s="9" t="s">
+      <c r="I21" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J21" s="11" t="s">
+      <c r="J21" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="K21" s="12" t="s">
+      <c r="K21" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="12" t="s">
+      <c r="A22" s="45"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="I22" s="12" t="s">
+      <c r="H22" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I22" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="J22" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K22" s="12" t="s">
+      <c r="K22" s="9" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="7" t="s">
+      <c r="A23" s="45"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I23" s="7" t="s">
+      <c r="H23" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J23" s="8" t="s">
+      <c r="J23" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K23" s="7" t="s">
+      <c r="K23" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+    </row>
+    <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="J25" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="K25" s="39" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1602,9 +1661,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1619,8 +1680,8 @@
     <col min="10" max="10" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="14"/>
       <c r="B1" t="s">
         <v>44</v>
       </c>
@@ -1628,8 +1689,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
       <c r="B2" t="s">
         <v>45</v>
       </c>
@@ -1637,27 +1698,27 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
       <c r="E3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1689,135 +1750,168 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="7" t="s">
+      <c r="G8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="9" t="s">
+    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="45"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="9" t="s">
+      <c r="G9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="37" t="s">
+    <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="45"/>
+      <c r="B10" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="12" t="s">
+      <c r="G10" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="15" t="s">
+    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="45"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="15" t="s">
+      <c r="G11" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="J11" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+    </row>
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="K13" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1852,7 +1946,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
+      <c r="A1" s="14"/>
       <c r="B1" t="s">
         <v>44</v>
       </c>
@@ -1861,30 +1955,30 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
+      <c r="A2" s="19"/>
       <c r="E2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
+      <c r="A3" s="19"/>
       <c r="E3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1919,78 +2013,78 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="9" t="s">
+      <c r="G8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="24" t="s">
+      <c r="A9" s="55"/>
+      <c r="B9" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="12" t="s">
+      <c r="G9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="9" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2021,7 +2115,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
+      <c r="A1" s="14"/>
       <c r="B1" t="s">
         <v>44</v>
       </c>
@@ -2030,31 +2124,31 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
+      <c r="A2" s="19"/>
       <c r="F2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
+      <c r="A3" s="19"/>
       <c r="F3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2092,85 +2186,85 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I8" s="9" t="s">
+      <c r="H8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="24" t="s">
+      <c r="A9" s="55"/>
+      <c r="B9" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="12" t="s">
+      <c r="H9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="9" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
[VM:Doug.Stearns@11/25/2014 2:57:30 PM] p13542 - ecl warnings for supervisors TTuser/items:Doug Stearns(stead1) Resolution for SCCB-S13542.DV.1: Add WARNING question in the eCoaching Log - Supervisor Module (FS) - Pending Development - Doug Stearns
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13836
</commit_message>
<xml_diff>
--- a/Requirements/status_email_notify.xlsx
+++ b/Requirements/status_email_notify.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="95">
   <si>
     <t>CSR</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>ETS</t>
+  </si>
+  <si>
+    <t>P13542 - eCL Warnings for SUP</t>
   </si>
 </sst>
 </file>
@@ -892,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E10"/>
+  <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,6 +1035,20 @@
         <v>76</v>
       </c>
     </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="29">
+        <v>41967</v>
+      </c>
+      <c r="C11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11">
+        <v>1.8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1041,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD25"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,50 +1678,50 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="50.28515625" customWidth="1"/>
-    <col min="10" max="10" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="50.28515625" customWidth="1"/>
+    <col min="11" max="11" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
       <c r="B1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" t="s">
         <v>45</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
         <v>17</v>
       </c>
@@ -1717,8 +1734,9 @@
       <c r="H6" s="46"/>
       <c r="I6" s="46"/>
       <c r="J6" s="46"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="46"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1726,199 +1744,249 @@
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="E8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="H8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="K8" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="45"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="50"/>
+      <c r="C9" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="H9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="J9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="K9" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="45"/>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="51"/>
+      <c r="C10" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="45"/>
+      <c r="B11" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="F11" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="9" t="s">
+      <c r="H11" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="J11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="K11" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="12" t="s">
+    <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="45"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="E12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="F12" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="G12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="12" t="s">
+      <c r="H12" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="J12" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="K12" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-    </row>
-    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B14" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="38" t="s">
+      <c r="C14" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="F14" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="39" t="s">
+      <c r="G14" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" s="39" t="s">
+      <c r="H14" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="I13" s="39" t="s">
+      <c r="J14" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="39" t="s">
+      <c r="K14" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="K13" s="3"/>
+      <c r="L14" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B8:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[VM:Doug.Stearns@12/19/2014 3:53:28 PM] p14031 - ecl ets non-comply report - initial prototype of req updates
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13873
</commit_message>
<xml_diff>
--- a/Requirements/status_email_notify.xlsx
+++ b/Requirements/status_email_notify.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="99">
   <si>
     <t>CSR</t>
   </si>
@@ -303,6 +303,20 @@
   </si>
   <si>
     <t>P13542 - eCL Warnings for SUP</t>
+  </si>
+  <si>
+    <t>ETS
+(OAE,OAM)</t>
+  </si>
+  <si>
+    <t>ETS
+(EOT,EA,HOL,ITD,ITI,FWH,HOLA,ITDA,ITIA,FWHA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A new eCoaching Log has been entered and requires your action. Please click on the link below to review and verify that the eCL entered on &lt;DATE&gt; for &lt;EMPLOYEE NAME&gt;  is a valid timecard infraction. Further directions are provided on the form. </t>
+  </si>
+  <si>
+    <t>P14031 - eCL ETS Non-compliance report</t>
   </si>
 </sst>
 </file>
@@ -463,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -557,6 +571,12 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -895,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E11"/>
+  <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,6 +1069,20 @@
         <v>76</v>
       </c>
     </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="29">
+        <v>41992</v>
+      </c>
+      <c r="C12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12">
+        <v>1.9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1056,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:D19"/>
+    <sheetView topLeftCell="G19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,19 +1138,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1154,10 +1188,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1189,8 +1223,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="48"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1220,8 +1254,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="48"/>
-      <c r="B10" s="50"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="12" t="s">
         <v>6</v>
       </c>
@@ -1251,8 +1285,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="50"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="9" t="s">
         <v>6</v>
       </c>
@@ -1282,8 +1316,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
-      <c r="B12" s="51"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="31" t="s">
         <v>10</v>
       </c>
@@ -1313,8 +1347,8 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
-      <c r="B13" s="49" t="s">
+      <c r="A13" s="50"/>
+      <c r="B13" s="51" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -1346,8 +1380,8 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
-      <c r="B14" s="50"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="4" t="s">
         <v>6</v>
       </c>
@@ -1390,19 +1424,19 @@
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="52" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="53" t="s">
+      <c r="C16" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="54" t="s">
+      <c r="E16" s="56" t="s">
         <v>55</v>
       </c>
       <c r="F16" s="38" t="s">
@@ -1425,11 +1459,11 @@
       </c>
     </row>
     <row r="17" spans="1:11" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="54"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="40" t="s">
         <v>60</v>
       </c>
@@ -1450,11 +1484,11 @@
       </c>
     </row>
     <row r="18" spans="1:11" s="19" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="54"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
       <c r="F18" s="42" t="s">
         <v>61</v>
       </c>
@@ -1475,11 +1509,11 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="54"/>
+      <c r="A19" s="47"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="56"/>
       <c r="F19" s="36" t="s">
         <v>59</v>
       </c>
@@ -1513,10 +1547,10 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="46" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -1548,8 +1582,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
-      <c r="B22" s="44"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="46"/>
       <c r="C22" s="9" t="s">
         <v>58</v>
       </c>
@@ -1579,8 +1613,8 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="45"/>
-      <c r="B23" s="44"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="46"/>
       <c r="C23" s="4" t="s">
         <v>58</v>
       </c>
@@ -1636,7 +1670,7 @@
         <v>58</v>
       </c>
       <c r="E25" s="39" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F25" s="39" t="s">
         <v>61</v>
@@ -1654,6 +1688,41 @@
         <v>43</v>
       </c>
       <c r="K25" s="39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="I26" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="J26" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="K26" s="41" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1678,17 +1747,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="3" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -1722,19 +1791,19 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1772,10 +1841,10 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="36" t="s">
@@ -1807,8 +1876,8 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="38" t="s">
         <v>6</v>
       </c>
@@ -1838,8 +1907,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
-      <c r="B10" s="51"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="53"/>
       <c r="C10" s="31" t="s">
         <v>10</v>
       </c>
@@ -1869,8 +1938,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
-      <c r="B11" s="44" t="s">
+      <c r="A11" s="47"/>
+      <c r="B11" s="46" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="40" t="s">
@@ -1902,8 +1971,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
-      <c r="B12" s="44"/>
+      <c r="A12" s="47"/>
+      <c r="B12" s="46"/>
       <c r="C12" s="12" t="s">
         <v>6</v>
       </c>
@@ -1958,8 +2027,8 @@
       <c r="D14" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="38" t="s">
-        <v>93</v>
+      <c r="E14" s="39" t="s">
+        <v>96</v>
       </c>
       <c r="F14" s="39" t="s">
         <v>64</v>
@@ -1980,6 +2049,42 @@
         <v>60</v>
       </c>
       <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="J15" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="K15" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2035,18 +2140,18 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2081,7 +2186,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="57" t="s">
         <v>70</v>
       </c>
       <c r="B8" s="21" t="s">
@@ -2113,7 +2218,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="55"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="21" t="s">
         <v>18</v>
       </c>
@@ -2204,19 +2309,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2254,7 +2359,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="57" t="s">
         <v>82</v>
       </c>
       <c r="B8" s="21" t="s">
@@ -2289,7 +2394,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="55"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="21" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
[VM:Doug.Stearns@1/7/2015 3:19:24 PM] p14031 - ecl ets non-comply report TTuser/items:Doug Stearns(stead1) Resolution for SCCB-S14031.DV.1: eCoaching - ETS Non-compliance action report (FS) - Pending Development - Doug Stearns
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13876
</commit_message>
<xml_diff>
--- a/Requirements/status_email_notify.xlsx
+++ b/Requirements/status_email_notify.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="101">
   <si>
     <t>CSR</t>
   </si>
@@ -305,18 +305,30 @@
     <t>P13542 - eCL Warnings for SUP</t>
   </si>
   <si>
+    <t>P14031 - eCL ETS Non-compliance report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A new eCoaching Log has been entered and requires your action. Please click on the link below to review and verify that the eCL entered on &lt;DATE&gt; for &lt;EMPLOYEE NAME&gt; is a valid timecard infraction. Further directions are provided on the form. </t>
+  </si>
+  <si>
     <t>ETS
-(OAE,OAM)</t>
+(OAE)
+Research Required</t>
   </si>
   <si>
     <t>ETS
-(EOT,EA,HOL,ITD,ITI,FWH,HOLA,ITDA,ITIA,FWHA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A new eCoaching Log has been entered and requires your action. Please click on the link below to review and verify that the eCL entered on &lt;DATE&gt; for &lt;EMPLOYEE NAME&gt;  is a valid timecard infraction. Further directions are provided on the form. </t>
-  </si>
-  <si>
-    <t>P14031 - eCL ETS Non-compliance report</t>
+(OAE,OAS)
+Research Required</t>
+  </si>
+  <si>
+    <t>ETS
+(EA,HOL,ITD,ITI,FWH)
+Opportunity</t>
+  </si>
+  <si>
+    <t>ETS
+(EOT,EA,HOLA,ITDA,ITIA,FWHA)
+Opportunity</t>
   </si>
 </sst>
 </file>
@@ -477,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -572,34 +584,31 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -918,7 +927,7 @@
   <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,10 +1080,10 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="29">
-        <v>41992</v>
+        <v>42002</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D12">
         <v>1.9</v>
@@ -1092,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="G19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,19 +1147,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1188,10 +1197,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="46" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1223,7 +1232,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="52"/>
       <c r="C9" s="4" t="s">
         <v>6</v>
@@ -1254,7 +1263,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="52"/>
       <c r="C10" s="12" t="s">
         <v>6</v>
@@ -1285,7 +1294,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="52"/>
       <c r="C11" s="9" t="s">
         <v>6</v>
@@ -1316,8 +1325,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="53"/>
+      <c r="A12" s="51"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="31" t="s">
         <v>10</v>
       </c>
@@ -1347,8 +1356,8 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
-      <c r="B13" s="51" t="s">
+      <c r="A13" s="51"/>
+      <c r="B13" s="46" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -1380,7 +1389,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="50"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="52"/>
       <c r="C14" s="4" t="s">
         <v>6</v>
@@ -1424,19 +1433,19 @@
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="54" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="55" t="s">
+      <c r="C16" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="56" t="s">
+      <c r="E16" s="55" t="s">
         <v>55</v>
       </c>
       <c r="F16" s="38" t="s">
@@ -1459,11 +1468,11 @@
       </c>
     </row>
     <row r="17" spans="1:11" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="56"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="55"/>
       <c r="F17" s="40" t="s">
         <v>60</v>
       </c>
@@ -1484,11 +1493,11 @@
       </c>
     </row>
     <row r="18" spans="1:11" s="19" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="55"/>
       <c r="F18" s="42" t="s">
         <v>61</v>
       </c>
@@ -1509,11 +1518,11 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="56"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="55"/>
       <c r="F19" s="36" t="s">
         <v>59</v>
       </c>
@@ -1547,10 +1556,10 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="48" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -1582,8 +1591,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="46"/>
+      <c r="A22" s="49"/>
+      <c r="B22" s="48"/>
       <c r="C22" s="9" t="s">
         <v>58</v>
       </c>
@@ -1613,8 +1622,8 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="46"/>
+      <c r="A23" s="49"/>
+      <c r="B23" s="48"/>
       <c r="C23" s="4" t="s">
         <v>58</v>
       </c>
@@ -1657,10 +1666,10 @@
       <c r="K24" s="20"/>
     </row>
     <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="46" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="38" t="s">
@@ -1670,7 +1679,7 @@
         <v>58</v>
       </c>
       <c r="E25" s="39" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F25" s="39" t="s">
         <v>61</v>
@@ -1692,12 +1701,8 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="B26" s="44" t="s">
-        <v>18</v>
-      </c>
+      <c r="A26" s="45"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="40" t="s">
         <v>58</v>
       </c>
@@ -1705,7 +1710,7 @@
         <v>58</v>
       </c>
       <c r="E26" s="41" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F26" s="41" t="s">
         <v>61</v>
@@ -1720,14 +1725,16 @@
         <v>36</v>
       </c>
       <c r="J26" s="41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K26" s="41" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A6:K6"/>
@@ -1749,15 +1756,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="3" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -1791,19 +1798,19 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1841,10 +1848,10 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="46" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="36" t="s">
@@ -1876,7 +1883,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="52"/>
       <c r="C9" s="38" t="s">
         <v>6</v>
@@ -1907,8 +1914,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="53"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="31" t="s">
         <v>10</v>
       </c>
@@ -1938,8 +1945,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="46" t="s">
+      <c r="A11" s="49"/>
+      <c r="B11" s="48" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="40" t="s">
@@ -1971,8 +1978,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
-      <c r="B12" s="46"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="12" t="s">
         <v>6</v>
       </c>
@@ -2015,10 +2022,10 @@
       <c r="K13" s="20"/>
     </row>
     <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="46" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="38" t="s">
@@ -2028,7 +2035,7 @@
         <v>58</v>
       </c>
       <c r="E14" s="39" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F14" s="39" t="s">
         <v>64</v>
@@ -2051,12 +2058,8 @@
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" s="44" t="s">
-        <v>18</v>
-      </c>
+      <c r="A15" s="45"/>
+      <c r="B15" s="47"/>
       <c r="C15" s="40" t="s">
         <v>58</v>
       </c>
@@ -2064,7 +2067,7 @@
         <v>58</v>
       </c>
       <c r="E15" s="41" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F15" s="41" t="s">
         <v>64</v>
@@ -2079,7 +2082,7 @@
         <v>35</v>
       </c>
       <c r="J15" s="41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K15" s="41" t="s">
         <v>60</v>
@@ -2087,11 +2090,13 @@
       <c r="L15" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2140,18 +2145,18 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2186,7 +2191,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="56" t="s">
         <v>70</v>
       </c>
       <c r="B8" s="21" t="s">
@@ -2218,7 +2223,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="57"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="21" t="s">
         <v>18</v>
       </c>
@@ -2309,19 +2314,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2359,7 +2364,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="56" t="s">
         <v>82</v>
       </c>
       <c r="B8" s="21" t="s">
@@ -2394,7 +2399,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="57"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="21" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
[VM:Doug.Stearns@3/20/2015 10:03:42 AM] p14512 - ecl training module - preliminary requirements TTuser/items:Doug Stearns(stead1) Resolution for SCCB-S14512.DV.1: eCoaching - Training module to be added to eCoaching - R&T - Pending Development - Doug Stearns
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13973
</commit_message>
<xml_diff>
--- a/Requirements/status_email_notify.xlsx
+++ b/Requirements/status_email_notify.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="11760" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="4" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Supervisor" sheetId="2" r:id="rId3"/>
     <sheet name="Quality" sheetId="3" r:id="rId4"/>
     <sheet name="LSA" sheetId="5" r:id="rId5"/>
+    <sheet name="Training" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="109">
   <si>
     <t>CSR</t>
   </si>
@@ -329,6 +330,30 @@
     <t>ETS
 (EOT,EA,HOLA,ITDA,ITIA,FWHA)
 Opportunity</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Trainer/Instructor, Training Supervisor, Training Manger</t>
+  </si>
+  <si>
+    <t>Employee (Trainer)</t>
+  </si>
+  <si>
+    <t>Training Supervisor</t>
+  </si>
+  <si>
+    <t>tbd</t>
+  </si>
+  <si>
+    <t>Training Manager</t>
+  </si>
+  <si>
+    <t>P14512 - eCL Training Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Level 1 Report - TBD</t>
   </si>
 </sst>
 </file>
@@ -369,7 +394,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -421,6 +446,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBFBBB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -489,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -584,6 +615,28 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -622,6 +675,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -629,6 +689,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFBFBBB"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -924,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E12"/>
+  <dimension ref="B2:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,6 +1157,20 @@
         <v>76</v>
       </c>
     </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="29">
+        <v>42079</v>
+      </c>
+      <c r="C13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="E13" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1101,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,19 +1226,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1197,10 +1276,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1232,8 +1311,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
-      <c r="B9" s="52"/>
+      <c r="A9" s="63"/>
+      <c r="B9" s="64"/>
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1263,8 +1342,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
-      <c r="B10" s="52"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="64"/>
       <c r="C10" s="12" t="s">
         <v>6</v>
       </c>
@@ -1294,8 +1373,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
-      <c r="B11" s="52"/>
+      <c r="A11" s="63"/>
+      <c r="B11" s="64"/>
       <c r="C11" s="9" t="s">
         <v>6</v>
       </c>
@@ -1325,8 +1404,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
-      <c r="B12" s="47"/>
+      <c r="A12" s="63"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="31" t="s">
         <v>10</v>
       </c>
@@ -1356,8 +1435,8 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
-      <c r="B13" s="46" t="s">
+      <c r="A13" s="63"/>
+      <c r="B13" s="58" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -1389,8 +1468,8 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
-      <c r="B14" s="52"/>
+      <c r="A14" s="63"/>
+      <c r="B14" s="64"/>
       <c r="C14" s="4" t="s">
         <v>6</v>
       </c>
@@ -1433,19 +1512,19 @@
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="53" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="54" t="s">
+      <c r="C16" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="55" t="s">
+      <c r="E16" s="67" t="s">
         <v>55</v>
       </c>
       <c r="F16" s="38" t="s">
@@ -1468,11 +1547,11 @@
       </c>
     </row>
     <row r="17" spans="1:11" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="55"/>
+      <c r="A17" s="61"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="67"/>
       <c r="F17" s="40" t="s">
         <v>60</v>
       </c>
@@ -1493,11 +1572,11 @@
       </c>
     </row>
     <row r="18" spans="1:11" s="19" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="55"/>
+      <c r="A18" s="61"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="67"/>
       <c r="F18" s="42" t="s">
         <v>61</v>
       </c>
@@ -1518,11 +1597,11 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="55"/>
+      <c r="A19" s="61"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="36" t="s">
         <v>59</v>
       </c>
@@ -1556,10 +1635,10 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="48" t="s">
+      <c r="B21" s="60" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -1591,8 +1670,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
-      <c r="B22" s="48"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="60"/>
       <c r="C22" s="9" t="s">
         <v>58</v>
       </c>
@@ -1622,8 +1701,8 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="48"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="60"/>
       <c r="C23" s="4" t="s">
         <v>58</v>
       </c>
@@ -1666,10 +1745,10 @@
       <c r="K24" s="20"/>
     </row>
     <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="B25" s="46" t="s">
+      <c r="B25" s="58" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="38" t="s">
@@ -1701,8 +1780,8 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
-      <c r="B26" s="47"/>
+      <c r="A26" s="57"/>
+      <c r="B26" s="59"/>
       <c r="C26" s="40" t="s">
         <v>58</v>
       </c>
@@ -1757,7 +1836,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1798,19 +1877,19 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1848,10 +1927,10 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="36" t="s">
@@ -1883,8 +1962,8 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
-      <c r="B9" s="52"/>
+      <c r="A9" s="61"/>
+      <c r="B9" s="64"/>
       <c r="C9" s="38" t="s">
         <v>6</v>
       </c>
@@ -1914,8 +1993,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
-      <c r="B10" s="47"/>
+      <c r="A10" s="61"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="31" t="s">
         <v>10</v>
       </c>
@@ -1945,8 +2024,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="48" t="s">
+      <c r="A11" s="61"/>
+      <c r="B11" s="60" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="40" t="s">
@@ -1978,8 +2057,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="48"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="12" t="s">
         <v>6</v>
       </c>
@@ -2022,10 +2101,10 @@
       <c r="K13" s="20"/>
     </row>
     <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="58" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="38" t="s">
@@ -2058,8 +2137,8 @@
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
-      <c r="B15" s="47"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="40" t="s">
         <v>58</v>
       </c>
@@ -2145,18 +2224,18 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2191,7 +2270,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="68" t="s">
         <v>70</v>
       </c>
       <c r="B8" s="21" t="s">
@@ -2223,7 +2302,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
+      <c r="A9" s="68"/>
       <c r="B9" s="21" t="s">
         <v>18</v>
       </c>
@@ -2314,19 +2393,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2364,7 +2443,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="68" t="s">
         <v>82</v>
       </c>
       <c r="B8" s="21" t="s">
@@ -2399,7 +2478,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
+      <c r="A9" s="68"/>
       <c r="B9" s="21" t="s">
         <v>18</v>
       </c>
@@ -2451,4 +2530,338 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="50.42578125" customWidth="1"/>
+    <col min="11" max="11" width="33" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="51"/>
+      <c r="B1" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="52"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="52"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="62" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="45" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="44" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="68" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="68"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="44" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="68"/>
+      <c r="B10" s="69" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" s="49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="68"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="53"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+    </row>
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="71" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="71" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tfs2470 - ecl mass log load (2482)
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C34167
</commit_message>
<xml_diff>
--- a/Requirements/status_email_notify.xlsx
+++ b/Requirements/status_email_notify.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Requirements\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="11760" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="4" r:id="rId1"/>
@@ -14,12 +19,12 @@
     <sheet name="LSA" sheetId="5" r:id="rId5"/>
     <sheet name="Training" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="113">
   <si>
     <t>CSR</t>
   </si>
@@ -184,9 +189,6 @@
   </si>
   <si>
     <t>A new eCoaching Log has been entered and requires your action. Please click on the link below to review and acknowledge the eCL entered on &lt;strong&gt;" &amp; Date &amp; "&lt;/strong&gt;" &amp; "Please click on the link below to review the eCoaching log.</t>
-  </si>
-  <si>
-    <t>strSource in feed file</t>
   </si>
   <si>
     <t xml:space="preserve">A new eCoaching Log has been entered on behalf of &lt;strong&gt;" &amp; strPerson &amp; "&lt;/strong&gt;"  on &lt;strong&gt;" &amp; DateTime.Now().ToString &amp; "&lt;/strong&gt; that requires your action. Please click on the link below  to review the eCoaching log. </t>
@@ -344,16 +346,37 @@
     <t>Training Supervisor</t>
   </si>
   <si>
-    <t>tbd</t>
-  </si>
-  <si>
     <t>Training Manager</t>
   </si>
   <si>
     <t>P14512 - eCL Training Module</t>
   </si>
   <si>
-    <t xml:space="preserve"> Level 1 Report - TBD</t>
+    <t>coded but not used</t>
+  </si>
+  <si>
+    <t>OMR
+(CAN,DFQ,OPN,ISQ,OSC,ACW,AHT,SPI,ACO,IDE,IEE,INF,ISG,NIT,RME,SLG,TRN,TR2,LCS)
+Research Required</t>
+  </si>
+  <si>
+    <t>OMR
+(IAE,IAT)
+Research Required</t>
+  </si>
+  <si>
+    <t>tfs2470 - eCL Mass log load</t>
+  </si>
+  <si>
+    <t>(SDR, ODT)
+Research Required</t>
+  </si>
+  <si>
+    <t>Generic</t>
+  </si>
+  <si>
+    <t>(OTH)
+Reinforcement</t>
   </si>
 </sst>
 </file>
@@ -394,7 +417,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -446,12 +469,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFBFBBB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -629,29 +646,34 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -670,18 +692,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,6 +727,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -745,7 +778,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -780,7 +813,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -989,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E13"/>
+  <dimension ref="B2:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,16 +1038,16 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="E2" s="22" t="s">
         <v>73</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -1022,13 +1055,13 @@
         <v>41869</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" s="26">
         <v>1</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -1036,13 +1069,13 @@
         <v>41891</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" s="26">
         <v>1.1000000000000001</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -1050,13 +1083,13 @@
         <v>41905</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5">
         <v>1.2</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -1064,13 +1097,13 @@
         <v>41908</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6">
         <v>1.3</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -1078,13 +1111,13 @@
         <v>41908</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D7">
         <v>1.4</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -1092,13 +1125,13 @@
         <v>41915</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D8">
         <v>1.5</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -1106,13 +1139,13 @@
         <v>41929</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9">
         <v>1.6</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -1120,13 +1153,13 @@
         <v>41942</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D10">
         <v>1.7</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -1134,13 +1167,13 @@
         <v>41967</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11">
         <v>1.8</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -1148,13 +1181,13 @@
         <v>42002</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D12">
         <v>1.9</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -1162,13 +1195,27 @@
         <v>42079</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D13">
         <v>1.1100000000000001</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="29">
+        <v>42471</v>
+      </c>
+      <c r="C14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="E14" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1178,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,7 +1251,7 @@
         <v>44</v>
       </c>
       <c r="F1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1213,32 +1260,32 @@
         <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="33"/>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1248,7 +1295,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>3</v>
@@ -1263,7 +1310,7 @@
         <v>8</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>33</v>
@@ -1276,10 +1323,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1298,7 +1345,7 @@
         <v>26</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>26</v>
@@ -1311,8 +1358,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="63"/>
-      <c r="B9" s="64"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1323,13 +1370,13 @@
         <v>11</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>35</v>
@@ -1338,12 +1385,12 @@
         <v>47</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="63"/>
-      <c r="B10" s="64"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="12" t="s">
         <v>6</v>
       </c>
@@ -1354,13 +1401,13 @@
         <v>13</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>32</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>37</v>
@@ -1373,8 +1420,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="63"/>
-      <c r="B11" s="64"/>
+      <c r="A11" s="64"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="9" t="s">
         <v>6</v>
       </c>
@@ -1385,13 +1432,13 @@
         <v>16</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>32</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>37</v>
@@ -1404,8 +1451,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="63"/>
-      <c r="B12" s="59"/>
+      <c r="A12" s="64"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="31" t="s">
         <v>10</v>
       </c>
@@ -1413,7 +1460,7 @@
         <v>6</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F12" s="31" t="s">
         <v>9</v>
@@ -1422,7 +1469,7 @@
         <v>26</v>
       </c>
       <c r="H12" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I12" s="31" t="s">
         <v>26</v>
@@ -1435,8 +1482,8 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="63"/>
-      <c r="B13" s="58" t="s">
+      <c r="A13" s="64"/>
+      <c r="B13" s="59" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -1449,27 +1496,27 @@
         <v>25</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>17</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>36</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="63"/>
-      <c r="B14" s="64"/>
+      <c r="A14" s="64"/>
+      <c r="B14" s="65"/>
       <c r="C14" s="4" t="s">
         <v>6</v>
       </c>
@@ -1480,13 +1527,13 @@
         <v>25</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>35</v>
@@ -1495,7 +1542,7 @@
         <v>48</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1512,104 +1559,108 @@
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="65" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="66" t="s">
+      <c r="C16" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="67" t="s">
-        <v>55</v>
+      <c r="E16" s="68" t="s">
+        <v>106</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G16" s="38" t="s">
         <v>32</v>
       </c>
       <c r="H16" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I16" s="38" t="s">
         <v>52</v>
       </c>
       <c r="J16" s="39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K16" s="40" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="61"/>
-      <c r="B17" s="60"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="67"/>
+      <c r="A17" s="62"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="69"/>
       <c r="F17" s="40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G17" s="40" t="s">
         <v>32</v>
       </c>
       <c r="H17" s="40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I17" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="J17" s="41" t="s">
         <v>89</v>
-      </c>
-      <c r="J17" s="41" t="s">
-        <v>90</v>
       </c>
       <c r="K17" s="40" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="19" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="61"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="67"/>
+      <c r="A18" s="62"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="56" t="s">
+        <v>108</v>
+      </c>
       <c r="F18" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G18" s="42" t="s">
         <v>17</v>
       </c>
       <c r="H18" s="42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I18" s="42" t="s">
         <v>36</v>
       </c>
       <c r="J18" s="43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K18" s="42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="61"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="67"/>
+      <c r="A19" s="62"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="55" t="s">
+        <v>107</v>
+      </c>
       <c r="F19" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G19" s="36" t="s">
         <v>12</v>
       </c>
       <c r="H19" s="36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I19" s="36" t="s">
         <v>35</v>
@@ -1618,7 +1669,7 @@
         <v>49</v>
       </c>
       <c r="K19" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1635,14 +1686,14 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="61" t="s">
+      <c r="A21" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="60" t="s">
+      <c r="B21" s="61" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>29</v>
@@ -1651,7 +1702,7 @@
         <v>53</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>32</v>
@@ -1670,10 +1721,10 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="61"/>
-      <c r="B22" s="60"/>
+      <c r="A22" s="62"/>
+      <c r="B22" s="61"/>
       <c r="C22" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>29</v>
@@ -1682,13 +1733,13 @@
         <v>28</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I22" s="9" t="s">
         <v>36</v>
@@ -1697,14 +1748,14 @@
         <v>43</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="61"/>
-      <c r="B23" s="60"/>
+      <c r="A23" s="62"/>
+      <c r="B23" s="61"/>
       <c r="C23" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>30</v>
@@ -1713,13 +1764,13 @@
         <v>28</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>35</v>
@@ -1728,7 +1779,7 @@
         <v>41</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1745,29 +1796,29 @@
       <c r="K24" s="20"/>
     </row>
     <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25" s="58" t="s">
+      <c r="A25" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="59" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E25" s="39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F25" s="39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G25" s="39" t="s">
         <v>17</v>
       </c>
       <c r="H25" s="39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I25" s="39" t="s">
         <v>36</v>
@@ -1776,38 +1827,108 @@
         <v>43</v>
       </c>
       <c r="K25" s="39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="58"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="41" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="57"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="F26" s="41" t="s">
-        <v>61</v>
       </c>
       <c r="G26" s="41" t="s">
         <v>17</v>
       </c>
       <c r="H26" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I26" s="41" t="s">
         <v>36</v>
       </c>
       <c r="J26" s="41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K26" s="41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="44" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="F28" s="46" t="s">
         <v>60</v>
+      </c>
+      <c r="G28" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="I28" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="J28" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="K28" s="46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="44" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="F30" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="G30" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="I30" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="J30" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="K30" s="46" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1824,7 +1945,7 @@
     <mergeCell ref="B16:B19"/>
     <mergeCell ref="C16:C19"/>
     <mergeCell ref="D16:D19"/>
-    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="E16:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1835,9 +1956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1858,7 +1977,7 @@
         <v>44</v>
       </c>
       <c r="F1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1867,29 +1986,32 @@
         <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="44" t="s">
+        <v>80</v>
+      </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1899,7 +2021,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>3</v>
@@ -1914,7 +2036,7 @@
         <v>8</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>33</v>
@@ -1927,10 +2049,10 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="36" t="s">
@@ -1943,13 +2065,13 @@
         <v>25</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>40</v>
@@ -1958,12 +2080,12 @@
         <v>41</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="61"/>
-      <c r="B9" s="64"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="38" t="s">
         <v>6</v>
       </c>
@@ -1974,13 +2096,13 @@
         <v>25</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>37</v>
@@ -1993,8 +2115,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="61"/>
-      <c r="B10" s="59"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="31" t="s">
         <v>10</v>
       </c>
@@ -2002,7 +2124,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F10" s="31" t="s">
         <v>9</v>
@@ -2011,7 +2133,7 @@
         <v>26</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I10" s="31" t="s">
         <v>26</v>
@@ -2024,8 +2146,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="61"/>
-      <c r="B11" s="60" t="s">
+      <c r="A11" s="62"/>
+      <c r="B11" s="61" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="40" t="s">
@@ -2038,13 +2160,13 @@
         <v>25</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>12</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>35</v>
@@ -2053,12 +2175,12 @@
         <v>39</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="61"/>
-      <c r="B12" s="60"/>
+      <c r="A12" s="62"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="12" t="s">
         <v>6</v>
       </c>
@@ -2069,13 +2191,13 @@
         <v>25</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>19</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I12" s="12" t="s">
         <v>40</v>
@@ -2084,7 +2206,7 @@
         <v>41</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2101,29 +2223,29 @@
       <c r="K13" s="20"/>
     </row>
     <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="B14" s="58" t="s">
+      <c r="A14" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="59" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" s="39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F14" s="39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G14" s="39" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I14" s="39" t="s">
         <v>35</v>
@@ -2132,39 +2254,39 @@
         <v>39</v>
       </c>
       <c r="K14" s="39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="57"/>
-      <c r="B15" s="59"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="60"/>
       <c r="C15" s="40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" s="41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F15" s="41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G15" s="41" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I15" s="41" t="s">
         <v>35</v>
       </c>
       <c r="J15" s="41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K15" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L15" s="3"/>
     </row>
@@ -2184,7 +2306,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2208,34 +2330,37 @@
         <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="44" t="s">
+        <v>80</v>
+      </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2257,7 +2382,7 @@
         <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>33</v>
@@ -2270,10 +2395,10 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="68" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="21" t="s">
+      <c r="A8" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="71" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -2283,13 +2408,13 @@
         <v>25</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>37</v>
@@ -2301,52 +2426,81 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="68"/>
-      <c r="B9" s="21" t="s">
+    <row r="9" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="70"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="70"/>
+      <c r="B10" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="9" t="s">
+      <c r="E10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="9" t="s">
+      <c r="G10" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I10" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
+      <c r="J10" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A6:J6"/>
-    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2354,7 +2508,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2377,35 +2531,38 @@
         <v>44</v>
       </c>
       <c r="F1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="44" t="s">
+        <v>80</v>
+      </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
+      <c r="A6" s="63" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2415,7 +2572,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>3</v>
@@ -2430,7 +2587,7 @@
         <v>8</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>33</v>
@@ -2443,10 +2600,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="68" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="21" t="s">
+      <c r="A8" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="71" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -2459,13 +2616,13 @@
         <v>25</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>37</v>
@@ -2477,56 +2634,88 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="68"/>
-      <c r="B9" s="21" t="s">
+    <row r="9" spans="1:11" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="70"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="70"/>
+      <c r="B10" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="9" t="s">
+      <c r="F10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J10" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K9" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
+      <c r="K10" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A6:K6"/>
-    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2536,15 +2725,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -2562,7 +2749,7 @@
       <c r="D1" s="44"/>
       <c r="E1" s="44"/>
       <c r="F1" s="44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G1" s="44"/>
       <c r="H1" s="44"/>
@@ -2571,13 +2758,15 @@
       <c r="K1" s="44"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="52"/>
-      <c r="B2" s="44"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="44" t="s">
+        <v>45</v>
+      </c>
       <c r="C2" s="44"/>
       <c r="D2" s="44"/>
       <c r="E2" s="44"/>
       <c r="F2" s="44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
@@ -2586,13 +2775,15 @@
       <c r="K2" s="44"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="52"/>
-      <c r="B3" s="44"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="44" t="s">
+        <v>80</v>
+      </c>
       <c r="C3" s="44"/>
       <c r="D3" s="44"/>
       <c r="E3" s="44"/>
       <c r="F3" s="44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G3" s="44"/>
       <c r="H3" s="44"/>
@@ -2627,19 +2818,19 @@
       <c r="K5" s="44"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
-        <v>101</v>
-      </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
+      <c r="A6" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="s">
@@ -2649,7 +2840,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" s="45" t="s">
         <v>3</v>
@@ -2664,7 +2855,7 @@
         <v>8</v>
       </c>
       <c r="H7" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I7" s="45" t="s">
         <v>33</v>
@@ -2677,14 +2868,14 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="44" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="68" t="s">
-        <v>102</v>
-      </c>
-      <c r="B8" s="69" t="s">
+      <c r="A8" s="70" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="71" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="46" t="s">
         <v>6</v>
@@ -2693,13 +2884,13 @@
         <v>25</v>
       </c>
       <c r="F8" s="46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G8" s="46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H8" s="46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I8" s="46" t="s">
         <v>37</v>
@@ -2712,10 +2903,10 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="68"/>
-      <c r="B9" s="69"/>
+      <c r="A9" s="70"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" s="36" t="s">
         <v>10</v>
@@ -2724,13 +2915,13 @@
         <v>25</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9" s="36" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H9" s="36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I9" s="36" t="s">
         <v>35</v>
@@ -2739,127 +2930,123 @@
         <v>41</v>
       </c>
       <c r="K9" s="36" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="44" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="68"/>
-      <c r="B10" s="69" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="70"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="44" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="70"/>
+      <c r="B11" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C11" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="70"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="49" t="s">
+      <c r="G12" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="H10" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="K10" s="49" t="s">
+      <c r="H12" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K12" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="68"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-    </row>
-    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="B13" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="70" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="70" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="71" t="s">
-        <v>105</v>
-      </c>
-      <c r="F13" s="71" t="s">
-        <v>61</v>
-      </c>
-      <c r="G13" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="71" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" s="71" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" s="71" t="s">
-        <v>43</v>
-      </c>
-      <c r="K13" s="71" t="s">
-        <v>60</v>
-      </c>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="52"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A6:K6"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B8:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>